<commit_message>
Integrated the simulation using random returns generated from history. Allowed for simulations with only an initial value and no subsequent cash flows.  Created some tests for the generation of historical random returns and a simulation that uses those.
</commit_message>
<xml_diff>
--- a/tests/testthat/data/siminput.xlsx
+++ b/tests/testthat/data/siminput.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b1bc217bf759e6b/aasim/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b1bc217bf759e6b/aasim/tests/testthat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BABC65FD-FAFB-4B12-8392-70BA5AC99B13}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B471062-4E4C-496D-80D3-91D51D402536}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="6405" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="6405" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="78">
   <si>
     <t>nTrials</t>
   </si>
@@ -227,6 +227,39 @@
   </si>
   <si>
     <t>p2ret-1</t>
+  </si>
+  <si>
+    <t>stockWt</t>
+  </si>
+  <si>
+    <t>nConsecMonths</t>
+  </si>
+  <si>
+    <t>retAdj</t>
+  </si>
+  <si>
+    <t>minDate</t>
+  </si>
+  <si>
+    <t>overrideInflation</t>
+  </si>
+  <si>
+    <t>asOfDate</t>
+  </si>
+  <si>
+    <t>randReturnType</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>maxDate</t>
+  </si>
+  <si>
+    <t>Hist1</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -546,10 +579,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -557,10 +590,11 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="19" width="15.46484375" customWidth="1"/>
+    <col min="29" max="29" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -595,49 +629,73 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="U1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="V1" t="s">
         <v>53</v>
       </c>
-      <c r="O1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="X1" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Y1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Z1" t="s">
         <v>50</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AB1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AC1" t="s">
         <v>54</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AD1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AE1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AF1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AG1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -671,32 +729,50 @@
       <c r="K2" t="b">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2">
+        <v>0.6</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>45547</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
+      <c r="U2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="1">
+      <c r="V2" s="1">
         <v>22102</v>
       </c>
-      <c r="O2" t="s">
+      <c r="W2" t="s">
         <v>23</v>
       </c>
-      <c r="P2">
+      <c r="X2">
         <v>65</v>
       </c>
-      <c r="Q2">
+      <c r="Y2">
         <v>1</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -730,50 +806,68 @@
       <c r="K3" t="b">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3">
+        <v>0.6</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>45547</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" t="s">
         <v>21</v>
       </c>
-      <c r="M3" t="s">
+      <c r="U3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="1">
+      <c r="V3" s="1">
         <v>22102</v>
       </c>
-      <c r="O3" t="s">
+      <c r="W3" t="s">
         <v>23</v>
       </c>
-      <c r="P3">
+      <c r="X3">
         <v>65</v>
       </c>
-      <c r="Q3">
+      <c r="Y3">
         <v>1</v>
       </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="s">
         <v>25</v>
       </c>
-      <c r="T3" t="s">
+      <c r="AB3" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="1">
+      <c r="AC3" s="1">
         <v>23182</v>
       </c>
-      <c r="V3" t="s">
+      <c r="AD3" t="s">
         <v>27</v>
       </c>
-      <c r="W3">
+      <c r="AE3">
         <v>65</v>
       </c>
-      <c r="X3">
+      <c r="AF3">
         <v>1</v>
       </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="AG3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -807,50 +901,68 @@
       <c r="K4" t="b">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4">
+        <v>0.6</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>45547</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T4" t="s">
         <v>21</v>
       </c>
-      <c r="M4" t="s">
+      <c r="U4" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="1">
+      <c r="V4" s="1">
         <v>22102</v>
       </c>
-      <c r="O4" t="s">
+      <c r="W4" t="s">
         <v>23</v>
       </c>
-      <c r="P4">
+      <c r="X4">
         <v>65</v>
       </c>
-      <c r="Q4">
+      <c r="Y4">
         <v>1</v>
       </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="s">
         <v>25</v>
       </c>
-      <c r="T4" t="s">
+      <c r="AB4" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="1">
+      <c r="AC4" s="1">
         <v>23182</v>
       </c>
-      <c r="V4" t="s">
+      <c r="AD4" t="s">
         <v>27</v>
       </c>
-      <c r="W4">
+      <c r="AE4">
         <v>65</v>
       </c>
-      <c r="X4">
+      <c r="AF4">
         <v>1</v>
       </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="AG4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -883,6 +995,77 @@
       </c>
       <c r="K5" t="b">
         <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0.6</v>
+      </c>
+      <c r="M5">
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>45547</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>500</v>
+      </c>
+      <c r="C6">
+        <v>1000000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>101</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0.6</v>
+      </c>
+      <c r="M6">
+        <v>12</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>44927</v>
+      </c>
+      <c r="P6" s="1">
+        <v>45291</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1">
+        <v>45547</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -895,8 +1078,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added functionality to simulate historical returns as they occurred (Chronological history).  Rather than drawing historical returns randomly, there is no an option to draw returns in sequence.  If a trial is 10 years, the first trial might be from Jan 26 - Dec 35 and the second from Feb 26 - Jan 36 and so on.
</commit_message>
<xml_diff>
--- a/tests/testthat/data/siminput.xlsx
+++ b/tests/testthat/data/siminput.xlsx
@@ -8,18 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b1bc217bf759e6b/aasim/tests/testthat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B471062-4E4C-496D-80D3-91D51D402536}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFB7D4A0-7E2D-4369-A030-F9A28AA6460D}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="6405" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="cashflows" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -579,10 +590,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AG6"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -591,6 +602,7 @@
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.46484375" bestFit="1" customWidth="1"/>
     <col min="12" max="19" width="15.46484375" customWidth="1"/>
+    <col min="22" max="22" width="9.19921875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1067,6 +1079,10 @@
       <c r="S6" s="1" t="s">
         <v>77</v>
       </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="S7" s="1"/>
+      <c r="V7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added print.sim function. Started an introductory vignette.  Modified some function names for clarity.
</commit_message>
<xml_diff>
--- a/tests/testthat/data/siminput.xlsx
+++ b/tests/testthat/data/siminput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b1bc217bf759e6b/aasim/tests/testthat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFB7D4A0-7E2D-4369-A030-F9A28AA6460D}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A4CB354-BF31-4264-BCAC-FB84BCA20AEA}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="82">
   <si>
     <t>nTrials</t>
   </si>
@@ -99,9 +99,6 @@
     <t>sim1</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>Rex</t>
   </si>
   <si>
@@ -258,9 +255,6 @@
     <t>asOfDate</t>
   </si>
   <si>
-    <t>randReturnType</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -271,6 +265,24 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>ChronHist1</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>John S</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>returnGeneratorMethod</t>
   </si>
 </sst>
 </file>
@@ -592,21 +604,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="12" max="19" width="15.46484375" customWidth="1"/>
-    <col min="22" max="22" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.31640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="19" width="15.453125" customWidth="1"/>
+    <col min="22" max="22" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -620,13 +632,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -641,28 +653,28 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" t="s">
         <v>67</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>68</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>69</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
         <v>70</v>
       </c>
-      <c r="P1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>71</v>
       </c>
-      <c r="R1" t="s">
-        <v>72</v>
-      </c>
       <c r="S1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="T1" t="s">
         <v>10</v>
@@ -671,19 +683,19 @@
         <v>11</v>
       </c>
       <c r="V1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W1" t="s">
         <v>12</v>
       </c>
       <c r="X1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y1" t="s">
         <v>13</v>
       </c>
       <c r="Z1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AA1" t="s">
         <v>14</v>
@@ -692,7 +704,7 @@
         <v>15</v>
       </c>
       <c r="AC1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AD1" t="s">
         <v>16</v>
@@ -704,10 +716,10 @@
         <v>18</v>
       </c>
       <c r="AG1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -718,7 +730,7 @@
         <v>1000000</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -757,19 +769,19 @@
         <v>45547</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
         <v>21</v>
-      </c>
-      <c r="U2" t="s">
-        <v>22</v>
       </c>
       <c r="V2" s="1">
         <v>22102</v>
       </c>
       <c r="W2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X2">
         <v>65</v>
@@ -784,9 +796,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>500</v>
@@ -795,7 +807,7 @@
         <v>1000000</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -834,19 +846,19 @@
         <v>45547</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U3" t="s">
         <v>21</v>
-      </c>
-      <c r="U3" t="s">
-        <v>22</v>
       </c>
       <c r="V3" s="1">
         <v>22102</v>
       </c>
       <c r="W3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X3">
         <v>65</v>
@@ -858,16 +870,16 @@
         <v>0</v>
       </c>
       <c r="AA3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB3" t="s">
         <v>25</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>26</v>
       </c>
       <c r="AC3" s="1">
         <v>23182</v>
       </c>
       <c r="AD3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AE3">
         <v>65</v>
@@ -879,9 +891,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -890,7 +902,7 @@
         <v>1000000</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -929,19 +941,19 @@
         <v>45547</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" t="s">
         <v>21</v>
-      </c>
-      <c r="U4" t="s">
-        <v>22</v>
       </c>
       <c r="V4" s="1">
         <v>22102</v>
       </c>
       <c r="W4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X4">
         <v>65</v>
@@ -953,16 +965,16 @@
         <v>0</v>
       </c>
       <c r="AA4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB4" t="s">
         <v>25</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>26</v>
       </c>
       <c r="AC4" s="1">
         <v>23182</v>
       </c>
       <c r="AD4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AE4">
         <v>65</v>
@@ -974,9 +986,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>500</v>
@@ -985,7 +997,7 @@
         <v>1000000</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -1024,12 +1036,12 @@
         <v>45547</v>
       </c>
       <c r="S5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>76</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -1038,7 +1050,7 @@
         <v>1000000</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -1077,12 +1089,76 @@
         <v>45547</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="S7" s="1"/>
-      <c r="V7" s="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7">
+        <v>500</v>
+      </c>
+      <c r="C7">
+        <v>1000000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>101</v>
+      </c>
+      <c r="G7">
+        <v>0.04</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0.6</v>
+      </c>
+      <c r="M7">
+        <v>12</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
+        <v>45547</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T7" t="s">
+        <v>78</v>
+      </c>
+      <c r="U7" t="s">
+        <v>79</v>
+      </c>
+      <c r="V7" s="1">
+        <v>21736</v>
+      </c>
+      <c r="W7" t="s">
+        <v>22</v>
+      </c>
+      <c r="X7">
+        <v>65</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1092,67 +1168,67 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2">
         <v>20000</v>
@@ -1164,27 +1240,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3">
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3">
         <v>5000</v>
@@ -1196,27 +1272,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
       </c>
       <c r="H4">
         <v>500</v>
@@ -1228,27 +1304,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H5">
         <v>50</v>
@@ -1260,27 +1336,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <v>10000</v>
@@ -1292,27 +1368,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7">
         <v>20000</v>
@@ -1324,27 +1400,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8">
         <v>100</v>
@@ -1356,27 +1432,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
         <v>56</v>
       </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H9">
         <v>100</v>
@@ -1388,27 +1464,27 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10">
         <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10">
         <v>70</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10">
         <v>200</v>
@@ -1420,27 +1496,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11">
         <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11">
         <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11">
         <v>300</v>
@@ -1452,27 +1528,27 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12">
         <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12">
         <v>400</v>
@@ -1484,27 +1560,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>62</v>
       </c>
       <c r="D13">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13">
         <v>4</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H13">
         <v>500</v>
@@ -1516,27 +1592,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14">
         <v>700</v>
@@ -1548,27 +1624,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15">
         <v>800</v>
@@ -1580,27 +1656,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16">
         <v>900</v>
@@ -1612,27 +1688,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H17">
         <v>1000</v>
@@ -1644,27 +1720,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
         <v>63</v>
       </c>
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18">
         <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18">
         <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H18">
         <v>40000</v>
@@ -1674,6 +1750,32 @@
       </c>
       <c r="J18">
         <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19">
+        <v>40000</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new charts.  Added function and calculation of IRRs for the trials.
</commit_message>
<xml_diff>
--- a/tests/testthat/data/siminput.xlsx
+++ b/tests/testthat/data/siminput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b1bc217bf759e6b/aasim/tests/testthat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="242" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A4CB354-BF31-4264-BCAC-FB84BCA20AEA}"/>
+  <xr:revisionPtr revIDLastSave="269" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB70A99B-D8FE-403F-B5EC-972C458954E9}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="84">
   <si>
     <t>nTrials</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>returnGeneratorMethod</t>
+  </si>
+  <si>
+    <t>Shiny1</t>
+  </si>
+  <si>
+    <t>Withdrawals</t>
   </si>
 </sst>
 </file>
@@ -602,23 +608,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AG7"/>
+  <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.31640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="19" width="15.453125" customWidth="1"/>
-    <col min="22" max="22" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.46484375" bestFit="1" customWidth="1"/>
+    <col min="12" max="19" width="15.46484375" customWidth="1"/>
+    <col min="22" max="22" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -719,7 +725,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -796,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -891,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -986,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1092,7 +1098,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -1158,6 +1164,60 @@
       </c>
       <c r="Z7">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8">
+        <v>500</v>
+      </c>
+      <c r="C8">
+        <v>1000000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>101</v>
+      </c>
+      <c r="G8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.08</v>
+      </c>
+      <c r="I8">
+        <v>0.09</v>
+      </c>
+      <c r="J8">
+        <v>0.01</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0.6</v>
+      </c>
+      <c r="M8">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45561</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1168,15 +1228,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1208,7 +1268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1240,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1272,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1304,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1336,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1368,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1400,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1432,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1464,7 +1524,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -1496,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1528,7 +1588,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1560,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1592,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1624,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1656,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1688,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1720,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1752,7 +1812,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1776,6 +1836,38 @@
       </c>
       <c r="J19">
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20">
+        <v>40000</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mostly bug fixes related to the calculation when the return generation method is "C", chronological.  Also fixed the geometric mean calculation.
</commit_message>
<xml_diff>
--- a/tests/testthat/data/siminput.xlsx
+++ b/tests/testthat/data/siminput.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="269" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB70A99B-D8FE-403F-B5EC-972C458954E9}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,8 +610,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="R8" s="1">
         <f ca="1">TODAY()</f>
-        <v>45561</v>
+        <v>45564</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>72</v>
@@ -1230,8 +1230,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added several new charts,
</commit_message>
<xml_diff>
--- a/tests/testthat/data/siminput.xlsx
+++ b/tests/testthat/data/siminput.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="269" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB70A99B-D8FE-403F-B5EC-972C458954E9}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57555" yWindow="12555" windowWidth="21600" windowHeight="4155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="R8" s="1">
         <f ca="1">TODAY()</f>
-        <v>45564</v>
+        <v>45579</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>72</v>

</xml_diff>